<commit_message>
(docs/requirements): update test cases
</commit_message>
<xml_diff>
--- a/docs/requirements/test_cases.xlsx
+++ b/docs/requirements/test_cases.xlsx
@@ -33,14 +33,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhCix5qVL+CwtkFdnK6UE5PyeRvpQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgMp6BJqXFYwjDYlMWNMPwPXOxQ0Q=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Planilla de Casos de Pruebas de Software</t>
   </si>
@@ -352,304 +352,6 @@
     <t>AchievementEvaluator, CriteriaValidator</t>
   </si>
   <si>
-    <t>CP-03</t>
-  </si>
-  <si>
-    <t>Error de conexión</t>
-  </si>
-  <si>
-    <t>Se interrumpe la conexión durante el desbloqueo</t>
-  </si>
-  <si>
-    <t>Gamification Service (Achievement Component + Celery Worker)</t>
-  </si>
-  <si>
-    <t>Manejo de errores</t>
-  </si>
-  <si>
-    <t>Interrupción duarante el proceso de desbloqueo</t>
-  </si>
-  <si>
-    <t>Celery reintenta automaticamente, no genera duplicidad de logro, conserva la consistencia de datos</t>
-  </si>
-  <si>
-    <t>Simular desconexión temporal de RabbitMQ y BD</t>
-  </si>
-  <si>
-    <t>Forzar caída del contenedor RabbitMQ o DB y monitorear reintento de Celery</t>
-  </si>
-  <si>
-    <t>Error controlado efectivamente, sin perdida de datos</t>
-  </si>
-  <si>
-    <t>El Worker reintenta correctamente a los 5 seg.</t>
-  </si>
-  <si>
-    <t>Infraestructura (RabbitMQ, PostgreSQL)</t>
-  </si>
-  <si>
-    <t>CP-04</t>
-  </si>
-  <si>
-    <t>Validación de puntos de experiencia</t>
-  </si>
-  <si>
-    <t>Verificar que al desbloquear un logro se acrediten los puntos correspondientes</t>
-  </si>
-  <si>
-    <t>XP Management Service</t>
-  </si>
-  <si>
-    <t>Asignación de puntos por logros</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Desbloqueo de logro con </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>reward_xp</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> &gt; 0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>RewardService.award_xp()</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> incrementa correctamente el XP en </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>UserStatistics</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">BD con usuario de XP conocido, conexión con </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>XPService</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> activa</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Consultar endpoint </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>/xp/user/{id}/</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> tras desbloqueo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">XP actualizado, </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>LevelUp</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> publicado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Integración con </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>XPService</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> validada</t>
-    </r>
-  </si>
-  <si>
-    <t>RewardService, XPService, UserStatistics</t>
-  </si>
-  <si>
-    <t>CP-05</t>
-  </si>
-  <si>
-    <t>Doble intento de desbloqueo</t>
-  </si>
-  <si>
-    <t>El usuario intenta desbloquear un logro ya obtenido</t>
-  </si>
-  <si>
-    <t>Prevención de duplicados en logros</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>TaskCompleted</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> event repetido</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>AchievementValidator.validate_not_already_unlocked()</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> detiene la acción, no se crean nuevos registros</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">Usuario con logro desbloqueado en </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>UserAchievement</t>
-    </r>
-  </si>
-  <si>
-    <t>Monitorear BD y logs después del segundo evento</t>
-  </si>
-  <si>
-    <t>Acción rechazada, sin duplicidad</t>
-  </si>
-  <si>
-    <t>Lógica de validación exitoso</t>
-  </si>
-  <si>
-    <t>AchievementValidator, AchievementService</t>
-  </si>
-  <si>
     <t>Descripción de la información a completar en cada columna</t>
   </si>
   <si>
@@ -820,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border/>
     <border>
       <left style="thin">
@@ -873,20 +575,36 @@
       </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+    </border>
+    <border>
+      <top style="thin">
         <color rgb="FF000000"/>
-      </bottom>
+      </top>
+    </border>
+    <border>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -941,15 +659,55 @@
     <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="2" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="6" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
@@ -1477,55 +1235,55 @@
       <c r="Z7" s="19"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="22">
         <v>45964.0</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="22">
         <v>45964.0</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="15" t="s">
+      <c r="Q8" s="23" t="s">
         <v>48</v>
       </c>
       <c r="R8" s="19"/>
@@ -1539,58 +1297,24 @@
       <c r="Z8" s="19"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="P9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="R9" s="19"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="31"/>
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
       <c r="U9" s="19"/>
@@ -1601,58 +1325,24 @@
       <c r="Z9" s="19"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="R10" s="19"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="31"/>
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
@@ -1663,58 +1353,24 @@
       <c r="Z10" s="19"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" s="14">
-        <v>45964.0</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q11" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="R11" s="19"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="31"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
@@ -1725,23 +1381,23 @@
       <c r="Z11" s="19"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
@@ -29437,7 +29093,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="23" t="str">
+      <c r="A1" s="37" t="str">
         <f>'Plantilla de Casos de Prueba'!A1</f>
         <v>Planilla de Casos de Pruebas de Software</v>
       </c>
@@ -29496,8 +29152,8 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>84</v>
+      <c r="A3" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -29526,11 +29182,11 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="25" t="s">
-        <v>85</v>
+      <c r="A4" s="39" t="s">
+        <v>50</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>86</v>
+      <c r="B4" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -29558,12 +29214,12 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="26" t="str">
+      <c r="A5" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!A6</f>
         <v>ID</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>87</v>
+      <c r="B5" s="40" t="s">
+        <v>52</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -29591,11 +29247,11 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>88</v>
+      <c r="B6" s="40" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -29623,12 +29279,12 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="26" t="str">
+      <c r="A7" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!C6</f>
         <v>Caso de Prueba</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>89</v>
+      <c r="B7" s="40" t="s">
+        <v>54</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -29656,12 +29312,12 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="26" t="str">
+      <c r="A8" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!D6</f>
         <v>Descripción</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>90</v>
+      <c r="B8" s="40" t="s">
+        <v>55</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -29689,12 +29345,12 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="26" t="str">
+      <c r="A9" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!E6</f>
         <v>Fecha</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>91</v>
+      <c r="B9" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -29722,12 +29378,12 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="26" t="str">
+      <c r="A10" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!F6</f>
         <v>Área Funcional / Sub proceso</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>92</v>
+      <c r="B10" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -29755,12 +29411,12 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="26" t="str">
+      <c r="A11" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!G6</f>
         <v>Funcionalidad / Característica</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>93</v>
+      <c r="B11" s="40" t="s">
+        <v>58</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -29788,12 +29444,12 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="26" t="str">
+      <c r="A12" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!H6</f>
         <v>Datos / Acciones de Entrada</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>94</v>
+      <c r="B12" s="40" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -29821,12 +29477,12 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="26" t="str">
+      <c r="A13" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!I6</f>
         <v>Resultado Esperado</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>95</v>
+      <c r="B13" s="40" t="s">
+        <v>60</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -29854,12 +29510,12 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="26" t="str">
+      <c r="A14" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!J6</f>
         <v>Requerimientos de Ambiente de Pruebas</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>96</v>
+      <c r="B14" s="40" t="s">
+        <v>61</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -29887,11 +29543,11 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="26" t="s">
-        <v>97</v>
+      <c r="A15" s="40" t="s">
+        <v>62</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>98</v>
+      <c r="B15" s="40" t="s">
+        <v>63</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -29919,12 +29575,12 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="26" t="str">
+      <c r="A16" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!L6</f>
         <v>Dependencias con otros casos de Prueba</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>99</v>
+      <c r="B16" s="40" t="s">
+        <v>64</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -29952,8 +29608,8 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="27" t="s">
-        <v>100</v>
+      <c r="A17" s="41" t="s">
+        <v>65</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -29982,12 +29638,12 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="26" t="str">
+      <c r="A18" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!M6</f>
         <v>Resultado Obtenido</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>101</v>
+      <c r="B18" s="40" t="s">
+        <v>66</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -30015,12 +29671,12 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="26" t="str">
+      <c r="A19" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!N6</f>
         <v>Estado</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>102</v>
+      <c r="B19" s="40" t="s">
+        <v>67</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -30048,12 +29704,12 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="26" t="str">
+      <c r="A20" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!O6</f>
         <v>Última Fecha de Estado</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>103</v>
+      <c r="B20" s="40" t="s">
+        <v>68</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -30081,12 +29737,12 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="26" t="str">
+      <c r="A21" s="40" t="str">
         <f>'Plantilla de Casos de Prueba'!P6</f>
         <v>Observaciones</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>104</v>
+      <c r="B21" s="40" t="s">
+        <v>69</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -30114,11 +29770,11 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>105</v>
+      <c r="B22" s="42" t="s">
+        <v>70</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>

</xml_diff>